<commit_message>
updated metadata for sampling
</commit_message>
<xml_diff>
--- a/Lab3/testdata.xlsx
+++ b/Lab3/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\Documents\Sensorer og instrumentering\SensorLab\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF658C77-21E7-40D9-9D5C-6AA8E6BE9437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D83113F-4D4B-4135-8B8B-8D2F8C4757CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{BF6DD6EF-F452-4794-8BC1-DACA4FFA8459}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>papir</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>145 til 119</t>
+  </si>
+  <si>
+    <t>Gode målinger</t>
+  </si>
+  <si>
+    <t>Feilmålinger av transmittans</t>
   </si>
 </sst>
 </file>
@@ -488,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213FF77B-D431-400E-A900-5E5D5B89E875}">
-  <dimension ref="B2:C40"/>
+  <dimension ref="B2:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -499,17 +505,17 @@
     <col min="2" max="2" width="29.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -517,83 +523,95 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12">
         <v>79</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="F12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="F13">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>8</v>
       </c>
@@ -601,7 +619,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>9</v>
       </c>
@@ -609,96 +627,108 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>8</v>
       </c>
       <c r="C30">
         <v>81</v>
       </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="F30">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>9</v>
       </c>
       <c r="C31">
         <v>97</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="F31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B33" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>8</v>
       </c>
       <c r="C39" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="F39">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>9</v>
       </c>
       <c r="C40">
         <v>97</v>
+      </c>
+      <c r="F40">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>